<commit_message>
Schedule and login, logout times
</commit_message>
<xml_diff>
--- a/Modelo DB bicirio.xlsx
+++ b/Modelo DB bicirio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trabajo\Somos Movilidad\bicirio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C567573-70DC-4DDA-AE37-257DB8237C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C469CF-3E20-40AF-8C1D-14A1D89158A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D12F0DD0-82F7-4372-9C9A-962D59EC70E5}"/>
   </bookViews>
@@ -922,7 +922,7 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1757,7 +1757,7 @@
   <dimension ref="A1:R50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12:T13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>